<commit_message>
updated Hf of FermMicrobe (results practically unchanged)
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/HP/data/HP_stacked_area_contributions_2021.3.7-13.11.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/HP/data/HP_stacked_area_contributions_2021.3.7-13.11.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\BioSTEAM 2.x.x\biorefineries\HP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\BioSTEAM 2.x.x\biorefineries\HP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5123DFE4-1E87-4DF9-B29F-46FC9EA551A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7B2116-89D9-40AD-BCC9-CD23670B46A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3732" yWindow="0" windowWidth="19308" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Heat utility" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="12">
   <si>
     <t>feedstock_group</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>MPSP</t>
+  </si>
+  <si>
+    <t>AOC material non-BT</t>
+  </si>
+  <si>
+    <t>AOC material BT</t>
   </si>
 </sst>
 </file>
@@ -97,7 +103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -120,15 +126,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,7 +502,7 @@
     <col min="1" max="1" width="27.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" s="1">
         <v>54.8</v>
       </c>
@@ -486,7 +510,7 @@
         <v>54.8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -524,7 +548,7 @@
         <v>0.21420601626380492</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -543,7 +567,7 @@
         <v>0.11918172538365</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -566,7 +590,7 @@
         <v>0.21052111136240992</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -585,7 +609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -599,8 +623,12 @@
         <f t="shared" si="0"/>
         <v>-0.70817835291582476</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <f>B7/(SUM($B$2:$B$9)-$B$8-$B$9-$B$7)</f>
+        <v>-0.41458103699006554</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -615,7 +643,7 @@
         <v>-1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -630,7 +658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -652,10 +680,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,7 +691,7 @@
     <col min="1" max="1" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" s="1">
         <v>54.8</v>
       </c>
@@ -671,7 +699,7 @@
         <v>54.8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -690,7 +718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -709,7 +737,7 @@
         <v>9.5329519516179476E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -728,7 +756,7 @@
         <v>0.2431321117208447</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -751,7 +779,7 @@
         <v>5.8339427414581743E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -770,7 +798,7 @@
         <v>9.0790701468241322E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -784,8 +812,12 @@
         <f t="shared" si="0"/>
         <v>-0.53973974186765006</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <f>B7/(SUM($B$2:$B$9)-$B$8-$B$9-$B$7)</f>
+        <v>-0.35053959262814427</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -800,7 +832,7 @@
         <v>3.6752244317171799E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -815,7 +847,7 @@
         <v>-0.8709855813504398</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -840,7 +872,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1001,7 +1033,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1159,15 +1191,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1311,6 +1344,24 @@
       <c r="E10">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <f>(SUM(B2:B10)-B8)*16953*350*24/1000000</f>
+        <v>143.49887951786584</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <f>(B8)*16953*350*24/1000000</f>
+        <v>6.333005983504898</v>
       </c>
     </row>
   </sheetData>

</xml_diff>